<commit_message>
using 1020 version benchmark report
</commit_message>
<xml_diff>
--- a/lib/report/benchmark_report/web14/exl/202006/jsliu__bank_test_&_city_(HF)(202006)_Management_Executive_Summary.xlsx
+++ b/lib/report/benchmark_report/web14/exl/202006/jsliu__bank_test_&_city_(HF)(202006)_Management_Executive_Summary.xlsx
@@ -137,7 +137,7 @@
     <t>As of date:Jun,2020</t>
   </si>
   <si>
-    <t>Printed on:2020-09-18 15:02</t>
+    <t>Printed on:2020-10-20 04:58</t>
   </si>
   <si>
     <t>REVIEW</t>
@@ -348,7 +348,7 @@
     <t>Percent of Assets</t>
   </si>
   <si>
-    <t>Bank*(Jun20)</t>
+    <t>Bank*(Dec19)</t>
   </si>
   <si>
     <t>Peer Group*(Dec18)</t>
@@ -399,7 +399,7 @@
     <t>Liquidity Ratio</t>
   </si>
   <si>
-    <t xml:space="preserve">Peer Group*: FFIEC [104M], Mutually-owned insured savings banks having assets less than $100 million, it has 96 banks, 96 banks have data  as of 12/31/2018.</t>
+    <t xml:space="preserve">Peer Group*: FFIEC [103M], Mutually-owned insured savings banks having assets between $100 million and $300 million, it has 97 banks, 97 banks have data  as of 12/31/2018.</t>
   </si>
   <si>
     <t>Equity to Assets</t>
@@ -619,7 +619,7 @@
     <t>Bubble Location: Comparing the Risk Adjusted Margin to the CECL rate.</t>
   </si>
   <si>
-    <t>Dupont Analysis(based on:Jun20)</t>
+    <t>Dupont Analysis(based on:Dec19)</t>
   </si>
   <si>
     <t>Notes:</t>
@@ -5980,7 +5980,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>$60,730</a:t>
+            <a:t>$113,237</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1100" b="1">
             <a:solidFill>
@@ -6068,8 +6068,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>0.27%
-$164</a:t>
+            <a:t>0.91%
+$1,029</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6149,8 +6149,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>0.00%
-$0</a:t>
+            <a:t>0.23%
+$266</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6230,8 +6230,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>0.27%
-$164</a:t>
+            <a:t>1.14%
+$1,295</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -6317,8 +6317,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>3.75%
-$2,275</a:t>
+            <a:t>4.23%
+$4,788</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -6404,8 +6404,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>0.58%
-$352</a:t>
+            <a:t>0.76%
+$858</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -6491,8 +6491,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>4.32%
-$2,626</a:t>
+            <a:t>4.99%
+$5,646</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -6578,8 +6578,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>0.00%
-$0</a:t>
+            <a:t>0.07%
+$74</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -6665,8 +6665,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>0.58%
-$352</a:t>
+            <a:t>0.76%
+$858</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -6926,8 +6926,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>-3.48%
--$2,111</a:t>
+            <a:t>-3.02%
+-$3,419</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -7013,8 +7013,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>0.49%
-$299</a:t>
+            <a:t>0.66%
+$746</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -7100,8 +7100,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>3.97%
-$2,410</a:t>
+            <a:t>3.68%
+$4,165</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -7187,8 +7187,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>0.01%
-$6</a:t>
+            <a:t>0.10%
+$109</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -7274,8 +7274,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>1.62%
-$982</a:t>
+            <a:t>0.09%
+$101</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -7361,8 +7361,8 @@
               </a:solidFill>
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
-            <a:t>2.69%
-$1,636</a:t>
+            <a:t>4.80%
+$5,437</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -7449,7 +7449,7 @@
               <a:latin typeface="Ubuntu"/>
             </a:rPr>
             <a:t>0.00%
-$3</a:t>
+$0</a:t>
           </a:r>
           <a:endParaRPr sz="1200" b="0">
             <a:solidFill>
@@ -9410,11 +9410,11 @@
       <c r="D25" s="46"/>
       <c r="E25" s="46"/>
       <c r="F25" s="68">
-        <v>0.00555753836740937</v>
+        <v>0.00961365318821152</v>
       </c>
       <c r="G25" s="49"/>
       <c r="H25" s="68">
-        <v>0.0032</v>
+        <v>0.0055</v>
       </c>
       <c r="I25" s="48"/>
       <c r="J25" s="48"/>
@@ -9423,11 +9423,11 @@
       </c>
       <c r="M25" s="46"/>
       <c r="N25" s="67">
-        <v>0.0279707731258491</v>
+        <v>0.0286483892867729</v>
       </c>
       <c r="O25" s="47"/>
       <c r="P25" s="67">
-        <v>0.00290666005</v>
+        <v>0.00564654599999999</v>
       </c>
       <c r="Q25" s="47"/>
       <c r="R25" s="47"/>
@@ -9439,11 +9439,11 @@
       <c r="D26" s="46"/>
       <c r="E26" s="46"/>
       <c r="F26" s="68">
-        <v>0.0257439773264053</v>
+        <v>0.0807834566240753</v>
       </c>
       <c r="G26" s="48"/>
       <c r="H26" s="68">
-        <v>0.0190280598947358</v>
+        <v>0.0363463894720236</v>
       </c>
       <c r="I26" s="48"/>
       <c r="J26" s="48"/>
@@ -9452,11 +9452,11 @@
       </c>
       <c r="M26" s="46"/>
       <c r="N26" s="67">
-        <v>0.434035179696184</v>
+        <v>0.00963902429695643</v>
       </c>
       <c r="O26" s="47"/>
       <c r="P26" s="67">
-        <v>0.0019841871</v>
+        <v>0.0031593996</v>
       </c>
       <c r="Q26" s="47"/>
       <c r="R26" s="47"/>
@@ -9468,11 +9468,11 @@
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="68">
-        <v>0.0350570417271868</v>
+        <v>0.0498457559020895</v>
       </c>
       <c r="G27" s="48"/>
       <c r="H27" s="69">
-        <v>0.0335</v>
+        <v>0.0333</v>
       </c>
       <c r="I27" s="51"/>
       <c r="J27" s="52"/>
@@ -9481,11 +9481,11 @@
       </c>
       <c r="M27" s="46"/>
       <c r="N27" s="67">
-        <v>0.112285136470298</v>
+        <v>0.014744012774787</v>
       </c>
       <c r="O27" s="47"/>
       <c r="P27" s="67">
-        <v>0.003183899225</v>
+        <v>0.00480099239999999</v>
       </c>
       <c r="Q27" s="47"/>
       <c r="R27" s="47"/>
@@ -9497,11 +9497,11 @@
       <c r="D28" s="46"/>
       <c r="E28" s="46"/>
       <c r="F28" s="68">
-        <v>0.0400772777910961</v>
+        <v>0.0575738622510097</v>
       </c>
       <c r="G28" s="49"/>
       <c r="H28" s="69">
-        <v>0.0409</v>
+        <v>0.0402</v>
       </c>
       <c r="I28" s="51"/>
       <c r="J28" s="52"/>
@@ -9510,11 +9510,11 @@
       </c>
       <c r="M28" s="46"/>
       <c r="N28" s="67">
-        <v>5.74348524144682E-05</v>
+        <v>0.00294432449488912</v>
       </c>
       <c r="O28" s="47"/>
       <c r="P28" s="67">
-        <v>0.103425253625</v>
+        <v>0.124393062</v>
       </c>
       <c r="Q28" s="47"/>
       <c r="R28" s="47"/>
@@ -9526,11 +9526,11 @@
       <c r="D29" s="46"/>
       <c r="E29" s="46"/>
       <c r="F29" s="68">
-        <v>0.0730526497795453</v>
+        <v>0.0627252279488234</v>
       </c>
       <c r="G29" s="49"/>
       <c r="H29" s="69">
-        <v>0.0494</v>
+        <v>0.0463</v>
       </c>
       <c r="I29" s="51"/>
       <c r="J29" s="52"/>
@@ -9539,11 +9539,11 @@
       </c>
       <c r="M29" s="46"/>
       <c r="N29" s="67">
-        <v>0.574348524144745</v>
+        <v>0.0559757508534055</v>
       </c>
       <c r="O29" s="47"/>
       <c r="P29" s="67">
-        <v>0.1115</v>
+        <v>0.138</v>
       </c>
       <c r="Q29" s="47"/>
       <c r="R29" s="47"/>
@@ -9555,11 +9555,11 @@
       <c r="D30" s="46"/>
       <c r="E30" s="46"/>
       <c r="F30" s="68">
-        <v>0.0253879360634698</v>
+        <v>0.0208158870678311</v>
       </c>
       <c r="G30" s="49"/>
       <c r="H30" s="68">
-        <v>0.0235</v>
+        <v>0.025</v>
       </c>
       <c r="I30" s="48"/>
       <c r="J30" s="48"/>
@@ -9571,11 +9571,11 @@
       <c r="D31" s="46"/>
       <c r="E31" s="46"/>
       <c r="F31" s="68">
-        <v>0.005589047977895</v>
+        <v>0.00791341916154665</v>
       </c>
       <c r="G31" s="49"/>
       <c r="H31" s="68">
-        <v>0.00853542545018776</v>
+        <v>0.00765896870304462</v>
       </c>
       <c r="I31" s="48"/>
       <c r="J31" s="48"/>
@@ -9587,11 +9587,11 @@
       <c r="D32" s="46"/>
       <c r="E32" s="46"/>
       <c r="F32" s="68">
-        <v>0.884728340675477</v>
+        <v>0.764500734214391</v>
       </c>
       <c r="G32" s="49"/>
       <c r="H32" s="68">
-        <v>0.8619</v>
+        <v>0.7849</v>
       </c>
       <c r="I32" s="48"/>
       <c r="J32" s="48"/>
@@ -9613,11 +9613,11 @@
       <c r="D33" s="46"/>
       <c r="E33" s="46"/>
       <c r="F33" s="68">
-        <v>0.15542577241899</v>
+        <v>0.0966761468487441</v>
       </c>
       <c r="G33" s="49"/>
       <c r="H33" s="69">
-        <v>0.148708750449046</v>
+        <v>0.0974456479602755</v>
       </c>
       <c r="I33" s="51"/>
       <c r="J33" s="52"/>
@@ -9640,11 +9640,11 @@
       <c r="D34" s="46"/>
       <c r="E34" s="46"/>
       <c r="F34" s="68">
-        <v>0.213338273434605</v>
+        <v>0.1191325384152</v>
       </c>
       <c r="G34" s="49"/>
       <c r="H34" s="69">
-        <v>0.168172689055141</v>
+        <v>0.151321770329717</v>
       </c>
       <c r="I34" s="51"/>
       <c r="J34" s="52"/>
@@ -9665,11 +9665,11 @@
       <c r="D35" s="46"/>
       <c r="E35" s="46"/>
       <c r="F35" s="68">
-        <v>0.303285167345931</v>
+        <v>0.837991604593569</v>
       </c>
       <c r="G35" s="49"/>
       <c r="H35" s="69">
-        <v>0.6707</v>
+        <v>0.690899999999999</v>
       </c>
       <c r="I35" s="51"/>
       <c r="J35" s="52"/>
@@ -9690,11 +9690,11 @@
       <c r="D36" s="46"/>
       <c r="E36" s="46"/>
       <c r="F36" s="68">
-        <v>1.4216163019567</v>
+        <v>7.03411188698932</v>
       </c>
       <c r="G36" s="49"/>
       <c r="H36" s="69">
-        <v>3.98816242856228</v>
+        <v>4.56576736113111</v>
       </c>
       <c r="I36" s="51"/>
       <c r="J36" s="52"/>
@@ -9715,11 +9715,11 @@
       <c r="D37" s="46"/>
       <c r="E37" s="46"/>
       <c r="F37" s="68">
-        <v>0.387236659518103</v>
+        <v>0.955172150712254</v>
       </c>
       <c r="G37" s="49"/>
       <c r="H37" s="69">
-        <v>0.820026898153808</v>
+        <v>0.820546318289788</v>
       </c>
       <c r="I37" s="51"/>
       <c r="J37" s="52"/>
@@ -9744,7 +9744,7 @@
       </c>
       <c r="G38" s="49"/>
       <c r="H38" s="69">
-        <v>0.032441302701338</v>
+        <v>0.0463526780166522</v>
       </c>
       <c r="I38" s="51"/>
       <c r="J38" s="52"/>
@@ -9764,11 +9764,11 @@
       <c r="D39" s="15"/>
       <c r="E39" s="16"/>
       <c r="F39" s="68">
-        <v>0</v>
+        <v>0.00593948149931776</v>
       </c>
       <c r="G39" s="49"/>
       <c r="H39" s="69">
-        <v>0.0220011942532882</v>
+        <v>0.0303987984675106</v>
       </c>
       <c r="I39" s="51"/>
       <c r="J39" s="52"/>
@@ -9916,16 +9916,16 @@
         <v>-0.415584415584416</v>
       </c>
       <c r="O46" s="72">
-        <v>0.000662410429420157</v>
+        <v>0.000662410425851592</v>
       </c>
       <c r="P46" s="72">
-        <v>-0.00525848848571022</v>
+        <v>-0.00525848850118264</v>
       </c>
       <c r="Q46" s="72">
-        <v>-0.0241983518646792</v>
+        <v>-0.024198351956217</v>
       </c>
       <c r="R46" s="72">
-        <v>-0.0277910534713925</v>
+        <v>-0.0277910533911993</v>
       </c>
     </row>
     <row r="47" ht="16.5" customHeight="1">
@@ -10216,19 +10216,19 @@
         <v>9900</v>
       </c>
       <c r="F55" s="71">
-        <v>9901.8880167298</v>
+        <v>9901.88801685563</v>
       </c>
       <c r="G55" s="71">
-        <v>9908.3818219098684</v>
+        <v>9908.38182188051</v>
       </c>
       <c r="H55" s="71">
-        <v>9901.48237178739</v>
+        <v>9901.48237138243</v>
       </c>
       <c r="I55" s="71">
-        <v>9877.7098477543113</v>
+        <v>9877.70984749698</v>
       </c>
       <c r="J55" s="71">
-        <v>9897.36551454534</v>
+        <v>9897.3655144038912</v>
       </c>
       <c r="K55" s="6"/>
       <c r="L55" s="46" t="s">
@@ -10354,19 +10354,19 @@
         <v>80969</v>
       </c>
       <c r="F58" s="71">
-        <v>80970.8880167298</v>
+        <v>80970.888016855592</v>
       </c>
       <c r="G58" s="71">
-        <v>80977.3818219098</v>
+        <v>80977.38182188051</v>
       </c>
       <c r="H58" s="71">
-        <v>80970.4823717874</v>
+        <v>80970.4823713824</v>
       </c>
       <c r="I58" s="71">
-        <v>80946.7098477543</v>
+        <v>80946.709847497</v>
       </c>
       <c r="J58" s="71">
-        <v>80966.365514545309</v>
+        <v>80966.3655144039</v>
       </c>
       <c r="K58" s="6"/>
       <c r="L58" s="46" t="s">
@@ -10400,19 +10400,19 @@
         <v>80961</v>
       </c>
       <c r="F59" s="71">
-        <v>80962.8880167298</v>
+        <v>80962.888016855592</v>
       </c>
       <c r="G59" s="71">
-        <v>80969.3818219098</v>
+        <v>80969.38182188051</v>
       </c>
       <c r="H59" s="71">
-        <v>80962.4823717874</v>
+        <v>80962.4823713824</v>
       </c>
       <c r="I59" s="71">
-        <v>80938.7098477543</v>
+        <v>80938.709847497</v>
       </c>
       <c r="J59" s="71">
-        <v>80958.365514545309</v>
+        <v>80958.3655144039</v>
       </c>
       <c r="K59" s="6"/>
       <c r="L59" s="46" t="s">
@@ -10446,19 +10446,19 @@
         <v>15973</v>
       </c>
       <c r="F60" s="71">
-        <v>15974.8880167298</v>
+        <v>15974.888016855599</v>
       </c>
       <c r="G60" s="71">
-        <v>15981.3818219098</v>
+        <v>15981.3818218805</v>
       </c>
       <c r="H60" s="71">
-        <v>15974.4823717874</v>
+        <v>15974.4823713824</v>
       </c>
       <c r="I60" s="71">
-        <v>15950.7098477543</v>
+        <v>15950.709847496999</v>
       </c>
       <c r="J60" s="71">
-        <v>15970.3655145453</v>
+        <v>15970.3655144039</v>
       </c>
       <c r="K60" s="6"/>
       <c r="L60" s="46" t="s">
@@ -10492,19 +10492,19 @@
         <v>0</v>
       </c>
       <c r="F61" s="71">
-        <v>612.440432573653</v>
+        <v>612.44043257362193</v>
       </c>
       <c r="G61" s="71">
-        <v>592.939574377001</v>
+        <v>592.93957437690608</v>
       </c>
       <c r="H61" s="71">
-        <v>566.557832044854</v>
+        <v>566.557832044548</v>
       </c>
       <c r="I61" s="71">
-        <v>542.755179894675</v>
+        <v>542.75517989458706</v>
       </c>
       <c r="J61" s="71">
-        <v>2314.69301889018</v>
+        <v>2314.69301888966</v>
       </c>
       <c r="K61" s="6"/>
       <c r="L61" s="46" t="s">
@@ -10538,19 +10538,19 @@
         <v>0</v>
       </c>
       <c r="F62" s="71">
-        <v>92.4246937275253</v>
+        <v>92.4246937276043</v>
       </c>
       <c r="G62" s="71">
-        <v>81.397449970029214</v>
+        <v>81.397449970016</v>
       </c>
       <c r="H62" s="71">
-        <v>72.7562664253824</v>
+        <v>72.756266425119392</v>
       </c>
       <c r="I62" s="71">
-        <v>63.6502659685598</v>
+        <v>63.6502659684317</v>
       </c>
       <c r="J62" s="71">
-        <v>310.228676091497</v>
+        <v>310.228676091171</v>
       </c>
       <c r="K62" s="6"/>
       <c r="L62" s="46" t="s">
@@ -10584,19 +10584,19 @@
         <v>0</v>
       </c>
       <c r="F63" s="71">
-        <v>520.015738846127</v>
+        <v>520.015738846017</v>
       </c>
       <c r="G63" s="71">
-        <v>511.54212440697097</v>
+        <v>511.54212440689</v>
       </c>
       <c r="H63" s="71">
-        <v>493.80156561947</v>
+        <v>493.80156561942897</v>
       </c>
       <c r="I63" s="71">
-        <v>479.10491392611397</v>
+        <v>479.104913926157</v>
       </c>
       <c r="J63" s="71">
-        <v>2004.46434279868</v>
+        <v>2004.4643427984902</v>
       </c>
       <c r="K63" s="6"/>
       <c r="L63" s="46" t="s">
@@ -10630,19 +10630,19 @@
         <v>0</v>
       </c>
       <c r="F64" s="71">
-        <v>7.51573884612843</v>
+        <v>7.51573884601897</v>
       </c>
       <c r="G64" s="71">
-        <v>-0.957875593027362</v>
+        <v>-0.957875593109464</v>
       </c>
       <c r="H64" s="71">
-        <v>-18.698434380528298</v>
+        <v>-18.698434380570298</v>
       </c>
       <c r="I64" s="71">
-        <v>-33.395086073885004</v>
+        <v>-33.395086073842805</v>
       </c>
       <c r="J64" s="71">
-        <v>-45.5356572013122</v>
+        <v>-45.5356572015036</v>
       </c>
       <c r="K64" s="6"/>
       <c r="L64" s="46" t="s">
@@ -11484,10 +11484,10 @@
         <v>21</v>
       </c>
       <c r="B2" s="2">
-        <v>1.921759753</v>
+        <v>1.8666168149</v>
       </c>
       <c r="C2" s="2">
-        <v>1.98818859</v>
+        <v>2.14180297</v>
       </c>
       <c r="D2" s="2">
         <v>10</v>

</xml_diff>